<commit_message>
Did some research for Metadata
</commit_message>
<xml_diff>
--- a/Understanding Data/Metadata - Vikash.xlsx
+++ b/Understanding Data/Metadata - Vikash.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABEACE02EC6B639863985BDE589E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1E46283B-2816-4FD4-A7AF-CECC63114F07}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABEACE02EC6B639863985BDE589E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9451B9B9-AAF9-42E4-AB5A-777DA63D641A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Comprehensive Species Tally</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Vikash, Edem, Harwinder</t>
+  </si>
+  <si>
+    <t>This is a Git Demo</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,7 +506,9 @@
       <c r="D2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>

</xml_diff>

<commit_message>
Added Understanding Data section for the data alotted to -Vikash
</commit_message>
<xml_diff>
--- a/Understanding Data/Metadata - Vikash.xlsx
+++ b/Understanding Data/Metadata - Vikash.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABEACE02EC6B639863985BDE589E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9451B9B9-AAF9-42E4-AB5A-777DA63D641A}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_F25DC773A252ABEACE02EC6B639863985BDE589E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5B7CA38E-CC25-4EAC-B15B-2337EC36F420}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Comprehensive Species Tally</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Vikash, Edem, Harwinder</t>
-  </si>
-  <si>
-    <t>This is a Git Demo</t>
   </si>
 </sst>
 </file>
@@ -464,7 +461,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,9 +503,7 @@
       <c r="D2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>

</xml_diff>

<commit_message>
Added consolidated files - Vikash
</commit_message>
<xml_diff>
--- a/Understanding Data/Metadata - Vikash.xlsx
+++ b/Understanding Data/Metadata - Vikash.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="117" documentId="11_F25DC773A252ABEACE02EC6B639863985BDE589E" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{181723B8-3295-4AA1-BDAE-8F5805301ABB}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="11_F25DC773A252ABEACE02EC6B639863985BDE589E" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{66C4BD7F-EECC-4671-91AF-68432A5474A1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Grids!$A$1:$B$294</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -509,7 +509,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -519,6 +519,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -572,6 +578,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -894,7 +906,7 @@
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="2"/>
@@ -957,7 +969,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="2"/>
@@ -985,7 +997,7 @@
       <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="2"/>
@@ -1011,7 +1023,7 @@
       <c r="C11" s="7">
         <v>2018</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="2"/>
@@ -3399,7 +3411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC1EE71-D454-4F11-8BE2-C8367360B30A}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>